<commit_message>
remove duplicate column that was used for testing
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/onehealth_biosample_package_template.xlsx
+++ b/assets/sample_metadata/onehealth_biosample_package_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E324062-668F-47CF-BC8B-EA08E45EF36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482D310D-E3EE-4EF4-BA37-898D76870E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="410">
   <si>
     <t>Strategy</t>
   </si>
@@ -1480,7 +1480,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1577,23 +1577,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC6C6C6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1746,9 +1735,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2063,10 +2049,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BB45"/>
+  <dimension ref="A1:BA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AX12" sqref="AX12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2093,10 +2079,9 @@
     <col min="42" max="50" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="51" max="52" width="13.453125" style="17" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="18.75" customHeight="1">
+    <row r="1" spans="1:53" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -2122,7 +2107,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="18.75" customHeight="1">
+    <row r="2" spans="1:53" ht="18.75" customHeight="1">
       <c r="A2" s="45" t="s">
         <v>388</v>
       </c>
@@ -2280,11 +2265,8 @@
       <c r="BA2" s="53" t="s">
         <v>409</v>
       </c>
-      <c r="BB2" s="54" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" ht="18.75" customHeight="1">
+    </row>
+    <row r="3" spans="1:53" ht="18.75" customHeight="1">
       <c r="A3" t="s">
         <v>402</v>
       </c>
@@ -2374,11 +2356,8 @@
       <c r="BA3" t="s">
         <v>408</v>
       </c>
-      <c r="BB3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" ht="18.75" customHeight="1">
+    </row>
+    <row r="4" spans="1:53" ht="18.75" customHeight="1">
       <c r="Y4" s="36"/>
       <c r="AC4" s="36"/>
       <c r="AE4" s="14"/>
@@ -2388,13 +2367,13 @@
       <c r="AR4" s="36"/>
       <c r="AZ4" s="49"/>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:53">
       <c r="Y5" s="36"/>
       <c r="AC5" s="36"/>
       <c r="AH5" s="36"/>
       <c r="AI5" s="36"/>
     </row>
-    <row r="6" spans="1:54" ht="18.75" customHeight="1">
+    <row r="6" spans="1:53" ht="18.75" customHeight="1">
       <c r="Y6" s="36"/>
       <c r="AC6" s="36"/>
       <c r="AE6" s="14"/>
@@ -2404,7 +2383,7 @@
       <c r="AR6" s="36"/>
       <c r="AZ6" s="50"/>
     </row>
-    <row r="7" spans="1:54" ht="18.75" customHeight="1">
+    <row r="7" spans="1:53" ht="18.75" customHeight="1">
       <c r="Y7" s="36"/>
       <c r="AC7" s="36"/>
       <c r="AE7" s="14"/>
@@ -2414,7 +2393,7 @@
       <c r="AR7" s="36"/>
       <c r="AY7" s="14"/>
     </row>
-    <row r="8" spans="1:54" ht="18.75" customHeight="1">
+    <row r="8" spans="1:53" ht="18.75" customHeight="1">
       <c r="Y8" s="36"/>
       <c r="AC8" s="36"/>
       <c r="AE8" s="14"/>
@@ -2423,7 +2402,7 @@
       <c r="AI8" s="36"/>
       <c r="AR8" s="36"/>
     </row>
-    <row r="9" spans="1:54" ht="18.75" customHeight="1">
+    <row r="9" spans="1:53" ht="18.75" customHeight="1">
       <c r="F9" s="13"/>
       <c r="M9" s="36"/>
       <c r="N9" s="46"/>
@@ -2434,7 +2413,7 @@
       <c r="AI9" s="36"/>
       <c r="AR9" s="36"/>
     </row>
-    <row r="10" spans="1:54" ht="18.75" customHeight="1">
+    <row r="10" spans="1:53" ht="18.75" customHeight="1">
       <c r="F10" s="13"/>
       <c r="M10" s="36"/>
       <c r="N10" s="46"/>
@@ -2445,7 +2424,7 @@
       <c r="AI10" s="36"/>
       <c r="AR10" s="36"/>
     </row>
-    <row r="11" spans="1:54" ht="18.75" customHeight="1">
+    <row r="11" spans="1:53" ht="18.75" customHeight="1">
       <c r="F11" s="13"/>
       <c r="M11" s="36"/>
       <c r="N11" s="46"/>
@@ -2456,7 +2435,7 @@
       <c r="AI11" s="36"/>
       <c r="AR11" s="36"/>
     </row>
-    <row r="12" spans="1:54" ht="18.75" customHeight="1">
+    <row r="12" spans="1:53" ht="18.75" customHeight="1">
       <c r="F12" s="13"/>
       <c r="M12" s="36"/>
       <c r="N12" s="46"/>
@@ -2467,7 +2446,7 @@
       <c r="AI12" s="36"/>
       <c r="AR12" s="36"/>
     </row>
-    <row r="13" spans="1:54" ht="18.75" customHeight="1">
+    <row r="13" spans="1:53" ht="18.75" customHeight="1">
       <c r="F13" s="13"/>
       <c r="M13" s="36"/>
       <c r="N13" s="46"/>
@@ -2478,7 +2457,7 @@
       <c r="AI13" s="36"/>
       <c r="AR13" s="36"/>
     </row>
-    <row r="14" spans="1:54" ht="18.75" customHeight="1">
+    <row r="14" spans="1:53" ht="18.75" customHeight="1">
       <c r="F14" s="13"/>
       <c r="M14" s="36"/>
       <c r="N14" s="46"/>
@@ -2489,7 +2468,7 @@
       <c r="AI14" s="36"/>
       <c r="AR14" s="36"/>
     </row>
-    <row r="15" spans="1:54" ht="18.75" customHeight="1">
+    <row r="15" spans="1:53" ht="18.75" customHeight="1">
       <c r="F15" s="13"/>
       <c r="M15" s="36"/>
       <c r="N15" s="46"/>
@@ -2500,7 +2479,7 @@
       <c r="AI15" s="36"/>
       <c r="AR15" s="36"/>
     </row>
-    <row r="16" spans="1:54" ht="18.75" customHeight="1">
+    <row r="16" spans="1:53" ht="18.75" customHeight="1">
       <c r="F16" s="13"/>
       <c r="M16" s="36"/>
       <c r="N16" s="46"/>
@@ -4669,8 +4648,8 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4684,10 +4663,10 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="56"/>
+      <c r="C2" s="55"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -4701,10 +4680,10 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="55"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4718,10 +4697,10 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="55"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -4735,10 +4714,10 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="55"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4752,10 +4731,10 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="55"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -4769,10 +4748,10 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="55"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -4786,10 +4765,10 @@
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="55"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -4803,10 +4782,10 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="55"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -4820,10 +4799,10 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="55"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -4837,10 +4816,10 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="55"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -4854,10 +4833,10 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="55"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -4871,10 +4850,10 @@
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="55"/>
+      <c r="C13" s="54"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -4888,10 +4867,10 @@
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="55"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -4905,10 +4884,10 @@
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="55"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -4922,10 +4901,10 @@
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="55"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -4939,10 +4918,10 @@
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="55"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -4956,10 +4935,10 @@
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="55"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -4973,10 +4952,10 @@
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="55"/>
+      <c r="C19" s="54"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -4990,10 +4969,10 @@
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="55"/>
+      <c r="C20" s="54"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -5007,10 +4986,10 @@
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="55" t="s">
+      <c r="B21" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="55"/>
+      <c r="C21" s="54"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -5024,10 +5003,10 @@
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="55"/>
+      <c r="C22" s="54"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -5041,10 +5020,10 @@
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="55"/>
+      <c r="C23" s="54"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -5058,10 +5037,10 @@
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="55"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -5271,10 +5250,10 @@
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="55"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -5286,8 +5265,8 @@
     </row>
     <row r="38" spans="1:11" ht="18.75" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -5301,10 +5280,10 @@
       <c r="A39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="56"/>
+      <c r="C39" s="55"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -5318,10 +5297,10 @@
       <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="55"/>
+      <c r="C40" s="54"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -5335,10 +5314,10 @@
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="55"/>
+      <c r="C41" s="54"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -5352,10 +5331,10 @@
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="55" t="s">
+      <c r="B42" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="55"/>
+      <c r="C42" s="54"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -5369,10 +5348,10 @@
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="55" t="s">
+      <c r="B43" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="55"/>
+      <c r="C43" s="54"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -5386,10 +5365,10 @@
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="55"/>
+      <c r="C44" s="54"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -5403,10 +5382,10 @@
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="55" t="s">
+      <c r="B45" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="55"/>
+      <c r="C45" s="54"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -5450,10 +5429,10 @@
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="55" t="s">
+      <c r="B48" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="55"/>
+      <c r="C48" s="54"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -5465,8 +5444,8 @@
     </row>
     <row r="49" spans="1:11" ht="18.75" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -5480,10 +5459,10 @@
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="55"/>
+      <c r="C50" s="54"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -5497,10 +5476,10 @@
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="55" t="s">
+      <c r="B51" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="55"/>
+      <c r="C51" s="54"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -5514,10 +5493,10 @@
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="55" t="s">
+      <c r="B52" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="55"/>
+      <c r="C52" s="54"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -5531,10 +5510,10 @@
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="55" t="s">
+      <c r="B53" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="55"/>
+      <c r="C53" s="54"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -5548,10 +5527,10 @@
       <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="55" t="s">
+      <c r="B54" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="55"/>
+      <c r="C54" s="54"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -5565,10 +5544,10 @@
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="55" t="s">
+      <c r="B55" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="55"/>
+      <c r="C55" s="54"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -5582,10 +5561,10 @@
       <c r="A56" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="55" t="s">
+      <c r="B56" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="55"/>
+      <c r="C56" s="54"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -5599,10 +5578,10 @@
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="55" t="s">
+      <c r="B57" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="55"/>
+      <c r="C57" s="54"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -5616,10 +5595,10 @@
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="55" t="s">
+      <c r="B58" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="55"/>
+      <c r="C58" s="54"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -5633,10 +5612,10 @@
       <c r="A59" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="55" t="s">
+      <c r="B59" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="55"/>
+      <c r="C59" s="54"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -5650,10 +5629,10 @@
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="55" t="s">
+      <c r="B60" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="55"/>
+      <c r="C60" s="54"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -5667,10 +5646,10 @@
       <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="55" t="s">
+      <c r="B61" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="55"/>
+      <c r="C61" s="54"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -5684,10 +5663,10 @@
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="55" t="s">
+      <c r="B62" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="C62" s="55"/>
+      <c r="C62" s="54"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -5701,10 +5680,10 @@
       <c r="A63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="55" t="s">
+      <c r="B63" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="55"/>
+      <c r="C63" s="54"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -5718,10 +5697,10 @@
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B64" s="55" t="s">
+      <c r="B64" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="55"/>
+      <c r="C64" s="54"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -5735,10 +5714,10 @@
       <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="55" t="s">
+      <c r="B65" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="55"/>
+      <c r="C65" s="54"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -5752,10 +5731,10 @@
       <c r="A66" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B66" s="55" t="s">
+      <c r="B66" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="55"/>
+      <c r="C66" s="54"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -5769,10 +5748,10 @@
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="55" t="s">
+      <c r="B67" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="55"/>
+      <c r="C67" s="54"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -5786,10 +5765,10 @@
       <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="55" t="s">
+      <c r="B68" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="55"/>
+      <c r="C68" s="54"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -5803,10 +5782,10 @@
       <c r="A69" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B69" s="55" t="s">
+      <c r="B69" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="C69" s="55"/>
+      <c r="C69" s="54"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -5820,10 +5799,10 @@
       <c r="A70" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="55" t="s">
+      <c r="B70" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="C70" s="55"/>
+      <c r="C70" s="54"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -5837,10 +5816,10 @@
       <c r="A71" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B71" s="55" t="s">
+      <c r="B71" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="C71" s="55"/>
+      <c r="C71" s="54"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -5854,10 +5833,10 @@
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="55" t="s">
+      <c r="B72" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="C72" s="55"/>
+      <c r="C72" s="54"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -5871,10 +5850,10 @@
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B73" s="55" t="s">
+      <c r="B73" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="55"/>
+      <c r="C73" s="54"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -5888,10 +5867,10 @@
       <c r="A74" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B74" s="55" t="s">
+      <c r="B74" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="C74" s="55"/>
+      <c r="C74" s="54"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -5905,10 +5884,10 @@
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="55" t="s">
+      <c r="B75" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="C75" s="55"/>
+      <c r="C75" s="54"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -5922,10 +5901,10 @@
       <c r="A76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B76" s="55" t="s">
+      <c r="B76" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="C76" s="55"/>
+      <c r="C76" s="54"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -5939,10 +5918,10 @@
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B77" s="55" t="s">
+      <c r="B77" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="55"/>
+      <c r="C77" s="54"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -6530,6 +6509,61 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -6538,61 +6572,6 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>